<commit_message>
SSP code chages for 2018-2019 Data
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201819.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XCD HR_Documents\Project Imp Documents\Regression Testing_2018_2019\Statutory_2018_19\Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="8" activeTab="10"/>
+    <workbookView activeTab="10" firstSheet="8" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetData" sheetId="14" r:id="rId2"/>
-    <sheet name="CreateFemaleEmployee" sheetId="2" r:id="rId3"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="6" r:id="rId4"/>
-    <sheet name="SmallEmployerRelief" sheetId="3" r:id="rId5"/>
-    <sheet name="ProcessPayrollForJulyMonthSAPP" sheetId="7" r:id="rId6"/>
-    <sheet name="ProcessPayrollForAugMonthSAPP" sheetId="8" r:id="rId7"/>
-    <sheet name="ProcessPayrollForSepMonthSAPP" sheetId="9" r:id="rId8"/>
-    <sheet name="CreateLeaveRequest" sheetId="10" r:id="rId9"/>
-    <sheet name="AverageWeeklyEarningsTestReport" sheetId="11" r:id="rId10"/>
-    <sheet name="ProcessPayrollForJan16MonthSAPP" sheetId="12" r:id="rId11"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetData" r:id="rId2" sheetId="14"/>
+    <sheet name="CreateFemaleEmployee" r:id="rId3" sheetId="2"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="6"/>
+    <sheet name="SmallEmployerRelief" r:id="rId5" sheetId="3"/>
+    <sheet name="ProcessPayrollForJulyMonthSAPP" r:id="rId6" sheetId="7"/>
+    <sheet name="ProcessPayrollForAugMonthSAPP" r:id="rId7" sheetId="8"/>
+    <sheet name="ProcessPayrollForSepMonthSAPP" r:id="rId8" sheetId="9"/>
+    <sheet name="CreateLeaveRequest" r:id="rId9" sheetId="10"/>
+    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="11"/>
+    <sheet name="ProcessPayrollForJan16MonthSAPP" r:id="rId11" sheetId="12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="188">
   <si>
     <t>TC</t>
   </si>
@@ -583,16 +583,23 @@
     <t>01/17/2019</t>
   </si>
   <si>
-    <t>January-2019</t>
-  </si>
-  <si>
     <t>DO NOT TOUCH SAAP2 Payments</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Week-1</t>
+  </si>
+  <si>
+    <t>January-2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -657,75 +664,75 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -742,10 +749,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -780,7 +787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -832,7 +839,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -937,7 +944,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -946,13 +953,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -962,7 +969,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -971,7 +978,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -980,7 +987,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -990,12 +997,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1026,7 +1033,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1045,7 +1052,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1057,19 +1064,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.11328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -1142,7 +1149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1156,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -1297,29 +1304,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1366,70 +1373,75 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="D2" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="25" t="s">
         <v>4</v>
       </c>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1476,7 +1488,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="63" r="2" s="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>169</v>
       </c>
@@ -1486,17 +1498,17 @@
       <c r="C2" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>184</v>
+      <c r="E2" s="24" t="s">
+        <v>187</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>173</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>174</v>
@@ -1518,15 +1530,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1535,8 +1547,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1559,7 +1571,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>146</v>
       </c>
@@ -1574,12 +1586,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView topLeftCell="AR1" workbookViewId="0">
@@ -1588,18 +1600,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="25" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="25.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -1980,15 +1992,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1997,12 +2009,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="43.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2031,7 +2043,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>146</v>
       </c>
@@ -2052,12 +2064,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2066,8 +2078,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2087,7 +2099,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="17.45" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>146</v>
       </c>
@@ -2099,13 +2111,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2114,18 +2126,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2172,7 +2184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>169</v>
       </c>
@@ -2212,14 +2224,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2228,17 +2240,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="5.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2285,7 +2297,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>169</v>
       </c>
@@ -2325,14 +2337,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2341,15 +2353,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2396,7 +2408,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.25" r="2" s="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>169</v>
       </c>
@@ -2436,14 +2448,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2452,15 +2464,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2534,6 +2546,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SAPP Leavecreate class code updates
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201819.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="191">
   <si>
     <t>TC</t>
   </si>
@@ -592,7 +592,16 @@
     <t>Week-1</t>
   </si>
   <si>
-    <t>January-2018</t>
+    <t>employeeTaxable</t>
+  </si>
+  <si>
+    <t>employeeNiable</t>
+  </si>
+  <si>
+    <t>includeInHolidayEarnings</t>
+  </si>
+  <si>
+    <t>January-2019</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1511,7 @@
         <v>96</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>173</v>
@@ -2456,10 +2465,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,9 +2482,11 @@
     <col min="7" max="7" customWidth="true" width="12.5703125" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -2504,16 +2515,25 @@
         <v>128</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>146</v>
       </c>
@@ -2541,9 +2561,20 @@
       <c r="I2" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="25" t="s">
         <v>4</v>
       </c>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>